<commit_message>
Added progress on chapter 13 to 16.
</commit_message>
<xml_diff>
--- a/progress.xlsx
+++ b/progress.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Idrici\Documents\04-project\05-AllOfStatistics\Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali Idrici\Documents\04-project\05-AllOfStatistics\AllOfStatistics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B65E8E-1BD5-4CAE-AB80-2F4E01378954}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E678AF8-14C0-4324-87FE-ED209BB9A4A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6885" yWindow="2850" windowWidth="20010" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="2160" windowWidth="22725" windowHeight="13110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="20">
   <si>
     <t>Done</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t xml:space="preserve">This is really hard. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">13.11 beta vector isn't the same as in the book </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Also, no notes were taken. </t>
   </si>
 </sst>
 </file>
@@ -352,7 +358,13 @@
                   <c:v>0.66666666666666663</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.54545454545454541</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.8571428571428571</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1384,14 +1396,14 @@
   <dimension ref="B2:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="28" width="15.7109375" customWidth="1"/>
+    <col min="4" max="28" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28" x14ac:dyDescent="0.25">
@@ -1550,7 +1562,15 @@
       </c>
       <c r="P3" s="4">
         <f>tracking!P4</f>
-        <v>0.54545454545454541</v>
+        <v>1</v>
+      </c>
+      <c r="Q3" s="4">
+        <f>tracking!Q4</f>
+        <v>1</v>
+      </c>
+      <c r="R3" s="4">
+        <f>tracking!R4</f>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
@@ -1590,6 +1610,12 @@
         <v>0</v>
       </c>
       <c r="P4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1637,6 +1663,12 @@
       <c r="P5" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="Q5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C6">
@@ -1678,6 +1710,12 @@
       <c r="P6" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="Q6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C7">
@@ -1720,6 +1758,12 @@
       <c r="P7" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="Q7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C8">
@@ -1757,7 +1801,15 @@
         <v>0</v>
       </c>
       <c r="O8" s="9"/>
-      <c r="P8" s="9"/>
+      <c r="P8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C9">
@@ -1794,6 +1846,12 @@
       <c r="P9" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="Q9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C10">
@@ -1830,6 +1888,7 @@
       <c r="P10" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="R10" s="3"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C11">
@@ -1858,7 +1917,9 @@
       <c r="M11" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P11" s="9"/>
+      <c r="P11" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C12">
@@ -1886,7 +1947,9 @@
       <c r="M12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P12" s="9"/>
+      <c r="P12" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C13">
@@ -1914,7 +1977,9 @@
       <c r="M13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="P13" s="9"/>
+      <c r="P13" s="3" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C14">
@@ -1935,7 +2000,9 @@
       <c r="M14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="P14" s="9"/>
+      <c r="P14" s="9" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.25">
       <c r="C15">
@@ -1981,7 +2048,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C17">
         <f t="shared" si="2"/>
         <v>14</v>
@@ -2003,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C18">
         <f t="shared" si="2"/>
         <v>15</v>
@@ -2023,7 +2090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C19">
         <f t="shared" si="2"/>
         <v>16</v>
@@ -2043,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C20">
         <f t="shared" si="2"/>
         <v>17</v>
@@ -2058,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C21">
         <f t="shared" si="2"/>
         <v>18</v>
@@ -2071,7 +2138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C22">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -2086,7 +2153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C23">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -2099,7 +2166,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -2114,7 +2181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -2126,7 +2193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -2144,7 +2211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F27" s="3" t="s">
         <v>0</v>
       </c>
@@ -2152,17 +2219,17 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
       <c r="N29" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
       <c r="F30" t="s">
         <v>10</v>
       </c>
@@ -2170,9 +2237,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="9:16" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
         <v>12</v>
+      </c>
+      <c r="P33" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -2186,8 +2261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797BF9C2-A3B4-4C3A-8786-51576B8F288F}">
   <dimension ref="C1:AB34"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="C1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2240,6 +2315,12 @@
       <c r="P1" s="1">
         <v>11</v>
       </c>
+      <c r="Q1" s="1">
+        <v>6</v>
+      </c>
+      <c r="R1" s="1">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
@@ -2286,7 +2367,7 @@
         <v>16</v>
       </c>
       <c r="N2">
-        <f t="shared" ref="N2:P2" si="1">SUM(N6:N31)</f>
+        <f t="shared" ref="N2:O2" si="1">SUM(N6:N31)</f>
         <v>7</v>
       </c>
       <c r="O2">
@@ -2294,7 +2375,15 @@
         <v>4</v>
       </c>
       <c r="P2">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="P2:R2" si="2">SUM(P6:P31)</f>
+        <v>11</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="R2">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
     </row>
@@ -2303,56 +2392,64 @@
         <v>7</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:P3" si="2">D1-D2</f>
+        <f t="shared" ref="D3:O3" si="3">D1-D2</f>
         <v>3</v>
       </c>
       <c r="E3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="F3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="G3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="H3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="I3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="K3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="M3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="O3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P3">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" ref="P3:R3" si="4">P1-P2</f>
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="4"/>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="3:28" x14ac:dyDescent="0.25">
@@ -2360,56 +2457,64 @@
         <v>1</v>
       </c>
       <c r="D4" s="5">
-        <f t="shared" ref="D4:P4" si="3">D2/D1</f>
+        <f t="shared" ref="D4:O4" si="5">D2/D1</f>
         <v>0.86956521739130432</v>
       </c>
       <c r="E4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.95238095238095233</v>
       </c>
       <c r="F4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.95833333333333337</v>
       </c>
       <c r="G4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.7142857142857143</v>
       </c>
       <c r="H4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.625</v>
       </c>
       <c r="I4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="J4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="K4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
       <c r="L4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.9</v>
       </c>
       <c r="M4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="N4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
       <c r="O4" s="5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.66666666666666663</v>
       </c>
       <c r="P4" s="5">
-        <f t="shared" si="3"/>
-        <v>0.54545454545454541</v>
+        <f t="shared" ref="P4:R4" si="6">P2/P1</f>
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" si="6"/>
+        <v>0.8571428571428571</v>
       </c>
     </row>
     <row r="5" spans="3:28" x14ac:dyDescent="0.25">
@@ -2418,35 +2523,35 @@
         <v>Chapter 1</v>
       </c>
       <c r="E5" s="1" t="str">
-        <f t="shared" ref="E5:L5" si="4">_xlfn.CONCAT("Chapter ", VALUE(RIGHT(D5,LEN(D5)-8))+1)</f>
+        <f t="shared" ref="E5:L5" si="7">_xlfn.CONCAT("Chapter ", VALUE(RIGHT(D5,LEN(D5)-8))+1)</f>
         <v>Chapter 2</v>
       </c>
       <c r="F5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Chapter 3</v>
       </c>
       <c r="G5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Chapter 4</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Chapter 5</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Chapter 6</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Chapter 7</v>
       </c>
       <c r="K5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Chapter 8</v>
       </c>
       <c r="L5" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>Chapter 9</v>
       </c>
       <c r="M5" s="1" t="str">
@@ -2454,63 +2559,63 @@
         <v>Chapter 10</v>
       </c>
       <c r="N5" s="1" t="str">
-        <f t="shared" ref="N5:AB5" si="5">_xlfn.CONCAT("Chapter ", VALUE(RIGHT(M5,LEN(M5)-8))+1)</f>
+        <f t="shared" ref="N5:AB5" si="8">_xlfn.CONCAT("Chapter ", VALUE(RIGHT(M5,LEN(M5)-8))+1)</f>
         <v>Chapter 11</v>
       </c>
       <c r="O5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 12</v>
       </c>
       <c r="P5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 13</v>
       </c>
       <c r="Q5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 14</v>
       </c>
       <c r="R5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 15</v>
       </c>
       <c r="S5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 16</v>
       </c>
       <c r="T5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 17</v>
       </c>
       <c r="U5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 18</v>
       </c>
       <c r="V5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 19</v>
       </c>
       <c r="W5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 20</v>
       </c>
       <c r="X5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 21</v>
       </c>
       <c r="Y5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 22</v>
       </c>
       <c r="Z5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 23</v>
       </c>
       <c r="AA5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 24</v>
       </c>
       <c r="AB5" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Chapter 25</v>
       </c>
     </row>
@@ -2570,10 +2675,18 @@
         <f>IF(main!P4="Done",1,0)</f>
         <v>1</v>
       </c>
+      <c r="Q6" s="2">
+        <f>IF(main!Q4="Done",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R6" s="2">
+        <f>IF(main!R4="Done",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C7">
-        <f t="shared" ref="C7:C29" si="6">C6+1</f>
+        <f t="shared" ref="C7:C29" si="9">C6+1</f>
         <v>2</v>
       </c>
       <c r="D7" s="2">
@@ -2628,10 +2741,18 @@
         <f>IF(main!P5="Done",1,0)</f>
         <v>1</v>
       </c>
+      <c r="Q7" s="2">
+        <f>IF(main!Q5="Done",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R7" s="2">
+        <f>IF(main!R5="Done",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="D8" s="2">
@@ -2686,10 +2807,18 @@
         <f>IF(main!P6="Done",1,0)</f>
         <v>1</v>
       </c>
+      <c r="Q8" s="2">
+        <f>IF(main!Q6="Done",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R8" s="2">
+        <f>IF(main!R6="Done",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="D9" s="2">
@@ -2740,10 +2869,18 @@
         <f>IF(main!P7="Done",1,0)</f>
         <v>1</v>
       </c>
+      <c r="Q9" s="2">
+        <f>IF(main!Q7="Done",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R9" s="2">
+        <f>IF(main!R7="Done",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="D10" s="2">
@@ -2792,12 +2929,20 @@
       </c>
       <c r="P10" s="2">
         <f>IF(main!P8="Done",1,0)</f>
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <f>IF(main!Q8="Done",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R10" s="2">
+        <f>IF(main!R8="Done",1,0)</f>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="D11" s="2">
@@ -2848,10 +2993,18 @@
         <f>IF(main!P9="Done",1,0)</f>
         <v>1</v>
       </c>
+      <c r="Q11" s="2">
+        <f>IF(main!Q9="Done",1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="R11" s="2">
+        <f>IF(main!R9="Done",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
       <c r="D12" s="2">
@@ -2898,10 +3051,14 @@
         <f>IF(main!P10="Done",1,0)</f>
         <v>1</v>
       </c>
+      <c r="R12" s="2">
+        <f>IF(main!R10="Done",1,0)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="D13" s="2">
@@ -2942,12 +3099,12 @@
       </c>
       <c r="P13" s="2">
         <f>IF(main!P11="Done",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
       <c r="D14" s="2">
@@ -2980,12 +3137,12 @@
       </c>
       <c r="P14" s="2">
         <f>IF(main!P12="Done",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="D15" s="2">
@@ -3018,12 +3175,12 @@
       </c>
       <c r="P15" s="2">
         <f>IF(main!P13="Done",1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
       <c r="D16" s="2">
@@ -3047,10 +3204,14 @@
         <f>IF(main!M14="Done",1,0)</f>
         <v>1</v>
       </c>
+      <c r="P16" s="2">
+        <f>IF(main!P14="Done",1,0)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
       <c r="D17" s="2">
@@ -3077,7 +3238,7 @@
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
       <c r="D18" s="2">
@@ -3104,7 +3265,7 @@
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
       <c r="D19" s="2">
@@ -3131,7 +3292,7 @@
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>15</v>
       </c>
       <c r="D20" s="2">
@@ -3158,7 +3319,7 @@
     </row>
     <row r="21" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>16</v>
       </c>
       <c r="D21" s="2">
@@ -3185,7 +3346,7 @@
     </row>
     <row r="22" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>17</v>
       </c>
       <c r="D22" s="2">
@@ -3203,7 +3364,7 @@
     </row>
     <row r="23" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>18</v>
       </c>
       <c r="D23" s="2">
@@ -3221,7 +3382,7 @@
     </row>
     <row r="24" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>19</v>
       </c>
       <c r="D24" s="2">
@@ -3239,7 +3400,7 @@
     </row>
     <row r="25" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="D25" s="2">
@@ -3257,7 +3418,7 @@
     </row>
     <row r="26" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>21</v>
       </c>
       <c r="D26" s="2">
@@ -3275,7 +3436,7 @@
     </row>
     <row r="27" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>22</v>
       </c>
       <c r="D27" s="2">
@@ -3289,7 +3450,7 @@
     </row>
     <row r="28" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="D28" s="2">
@@ -3303,7 +3464,7 @@
     </row>
     <row r="29" spans="3:13" x14ac:dyDescent="0.25">
       <c r="C29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>24</v>
       </c>
       <c r="F29" s="2">
@@ -3317,18 +3478,18 @@
       </c>
       <c r="E32" s="1">
         <f>SUM(D2:AB2)</f>
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G32" s="1">
         <f>SUM(D1:AB1)</f>
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="I32" s="1">
         <f>E32/G32</f>
-        <v>0.85889570552147243</v>
+        <v>0.89204545454545459</v>
       </c>
     </row>
     <row r="34" spans="4:5" x14ac:dyDescent="0.25">
@@ -3337,7 +3498,7 @@
       </c>
       <c r="E34" s="1">
         <f>G32-E32</f>
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>